<commit_message>
Rename frontend-simplified to frontend for cleaner structure
</commit_message>
<xml_diff>
--- a/backend/Log.xlsx
+++ b/backend/Log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1348,6 +1348,406 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1754583810409</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:30.409</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Apply Button Pressed</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>{'taskMode': 'First: Yellow', 'taskOrder': 'Free'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1754583810907</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:30.907</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Initialize Robot Button Pressed</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1754583816966</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:36.966</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>{'taskId': '1', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1754583817031</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.031</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>{'taskId': '2', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1754583817100</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.100</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>{'taskId': '3', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1754583817165</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.165</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>{'taskId': '5', 'assignedTo': 'Robot', 'sliderValue': 10}</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1754583817307</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.307</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>{'taskId': '6', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1754583817428</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.428</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>{'taskId': '8', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1754583817542</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.542</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>{'taskId': '9', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1754583817642</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.642</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>{'taskId': '10', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1754583817942</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:37.942</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>{'taskId': '12', 'assignedTo': 'Human', 'sliderValue': 2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1754583818818</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:38.818</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>{'taskId': '14', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1754583819569</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:39.569</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>{'taskId': '15', 'assignedTo': 'Human', 'sliderValue': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1754583820610</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:40.610</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Task Allocation Changed</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>{'taskId': '18', 'assignedTo': 'Human', 'sliderValue': 0}</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>P76</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1754583822249</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:42.249</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Start Button Pressed</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Robot</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1754583839907</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2025-08-07 18:23:59.907</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Robot Task Completed</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>{'task_name': 'Bridge_triangle_roof', 'urp_name': 'Bridge_triangle_roof'}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>